<commit_message>
Move CH4 oxidation to other soil properties
</commit_message>
<xml_diff>
--- a/data/normative-effects.xlsx
+++ b/data/normative-effects.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephen.wood/Box Sync/Work/The Nature Conservancy/Global Soils/AgEvidence/code-and-data/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69C305A4-2BE9-C345-B6DF-AE550CB27206}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4122DAAD-04F3-184A-9425-D4D4E66EC2F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2520" yWindow="460" windowWidth="19200" windowHeight="14560" xr2:uid="{E2614878-5E79-439B-BF47-44ECB7DBED54}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$K$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$K$210</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1363" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1369" uniqueCount="213">
   <si>
     <t>Review</t>
   </si>
@@ -664,6 +664,9 @@
   </si>
   <si>
     <t>Pest Management</t>
+  </si>
+  <si>
+    <t>Methane oxidation</t>
   </si>
 </sst>
 </file>
@@ -725,7 +728,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -798,13 +801,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
@@ -885,6 +899,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1201,12 +1218,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5790928A-FDEF-4501-A63F-C28CBDB4D383}">
-  <dimension ref="A1:K209"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:K210"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A158" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="E175" sqref="E175"/>
+      <selection pane="bottomLeft" activeCell="F210" sqref="F210"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1328,7 +1346,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
         <v>190</v>
       </c>
@@ -1349,7 +1367,7 @@
       </c>
       <c r="G5" s="36"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
         <v>190</v>
       </c>
@@ -1391,7 +1409,7 @@
       </c>
       <c r="G7" s="36"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
         <v>190</v>
       </c>
@@ -1444,7 +1462,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>190</v>
       </c>
@@ -1465,7 +1483,7 @@
       </c>
       <c r="G10" s="36"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
         <v>190</v>
       </c>
@@ -1486,7 +1504,7 @@
       </c>
       <c r="G11" s="36"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
         <v>190</v>
       </c>
@@ -1507,7 +1525,7 @@
       </c>
       <c r="G12" s="36"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
         <v>190</v>
       </c>
@@ -1528,7 +1546,7 @@
       </c>
       <c r="G13" s="36"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
         <v>190</v>
       </c>
@@ -1549,7 +1567,7 @@
       </c>
       <c r="G14" s="36"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
         <v>190</v>
       </c>
@@ -1570,7 +1588,7 @@
       </c>
       <c r="G15" s="36"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
         <v>190</v>
       </c>
@@ -1602,7 +1620,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
         <v>190</v>
       </c>
@@ -1623,7 +1641,7 @@
       </c>
       <c r="G17" s="36"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="11" t="s">
         <v>190</v>
       </c>
@@ -1686,7 +1704,7 @@
       </c>
       <c r="G20" s="36"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
         <v>190</v>
       </c>
@@ -1707,7 +1725,7 @@
       </c>
       <c r="G21" s="36"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
         <v>190</v>
       </c>
@@ -1728,7 +1746,7 @@
       </c>
       <c r="G22" s="36"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="11" t="s">
         <v>190</v>
       </c>
@@ -1749,7 +1767,7 @@
       </c>
       <c r="G23" s="36"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="11" t="s">
         <v>190</v>
       </c>
@@ -1770,7 +1788,7 @@
       </c>
       <c r="G24" s="36"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="11" t="s">
         <v>190</v>
       </c>
@@ -1791,7 +1809,7 @@
       </c>
       <c r="G25" s="36"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
         <v>190</v>
       </c>
@@ -1812,7 +1830,7 @@
       </c>
       <c r="G26" s="36"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="11" t="s">
         <v>190</v>
       </c>
@@ -1844,7 +1862,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="11" t="s">
         <v>190</v>
       </c>
@@ -1897,7 +1915,7 @@
       </c>
       <c r="G29" s="36"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="11" t="s">
         <v>190</v>
       </c>
@@ -1918,7 +1936,7 @@
       </c>
       <c r="G30" s="36"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
         <v>190</v>
       </c>
@@ -1939,7 +1957,7 @@
       </c>
       <c r="G31" s="36"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
         <v>190</v>
       </c>
@@ -1960,7 +1978,7 @@
       </c>
       <c r="G32" s="36"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="11" t="s">
         <v>190</v>
       </c>
@@ -2002,7 +2020,7 @@
       </c>
       <c r="G34" s="36"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="11" t="s">
         <v>190</v>
       </c>
@@ -2023,7 +2041,7 @@
       </c>
       <c r="G35" s="36"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="11" t="s">
         <v>190</v>
       </c>
@@ -2044,7 +2062,7 @@
       </c>
       <c r="G36" s="36"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="11" t="s">
         <v>190</v>
       </c>
@@ -2065,7 +2083,7 @@
       </c>
       <c r="G37" s="36"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="11" t="s">
         <v>190</v>
       </c>
@@ -2107,7 +2125,7 @@
       </c>
       <c r="G39" s="36"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="11" t="s">
         <v>190</v>
       </c>
@@ -2194,7 +2212,7 @@
       </c>
       <c r="G43" s="36"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="11" t="s">
         <v>190</v>
       </c>
@@ -2281,7 +2299,7 @@
       <c r="G46" s="36"/>
       <c r="K46" s="12"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" s="11" t="s">
         <v>190</v>
       </c>
@@ -2303,7 +2321,7 @@
       <c r="G47" s="36"/>
       <c r="K47" s="12"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" s="11" t="s">
         <v>190</v>
       </c>
@@ -2324,7 +2342,7 @@
       </c>
       <c r="G48" s="36"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" s="11" t="s">
         <v>190</v>
       </c>
@@ -2345,7 +2363,7 @@
       </c>
       <c r="G49" s="36"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" s="11" t="s">
         <v>190</v>
       </c>
@@ -2366,7 +2384,7 @@
       </c>
       <c r="G50" s="36"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" s="11" t="s">
         <v>190</v>
       </c>
@@ -2387,7 +2405,7 @@
       </c>
       <c r="G51" s="36"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" s="11" t="s">
         <v>190</v>
       </c>
@@ -2429,7 +2447,7 @@
       </c>
       <c r="G53" s="36"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" s="11" t="s">
         <v>190</v>
       </c>
@@ -2475,7 +2493,7 @@
       <c r="H55" s="40"/>
       <c r="I55" s="40"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" s="11" t="s">
         <v>190</v>
       </c>
@@ -2498,7 +2516,7 @@
       <c r="H56" s="40"/>
       <c r="I56" s="40"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" s="11" t="s">
         <v>190</v>
       </c>
@@ -2523,7 +2541,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" s="11" t="s">
         <v>190</v>
       </c>
@@ -2546,7 +2564,7 @@
       <c r="I58" s="40"/>
       <c r="K58" s="15"/>
     </row>
-    <row r="59" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" s="11" t="s">
         <v>190</v>
       </c>
@@ -2567,7 +2585,7 @@
       </c>
       <c r="G59" s="41"/>
     </row>
-    <row r="60" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:11" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" s="11" t="s">
         <v>190</v>
       </c>
@@ -2599,7 +2617,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
         <v>211</v>
       </c>
@@ -2620,7 +2638,7 @@
       </c>
       <c r="G61" s="36"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
         <v>211</v>
       </c>
@@ -2641,7 +2659,7 @@
       </c>
       <c r="G62" s="36"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
         <v>211</v>
       </c>
@@ -2662,7 +2680,7 @@
       </c>
       <c r="G63" s="36"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
         <v>211</v>
       </c>
@@ -2683,7 +2701,7 @@
       </c>
       <c r="G64" s="36"/>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
         <v>211</v>
       </c>
@@ -2704,7 +2722,7 @@
       </c>
       <c r="G65" s="36"/>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
         <v>211</v>
       </c>
@@ -2725,7 +2743,7 @@
       </c>
       <c r="G66" s="36"/>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
         <v>211</v>
       </c>
@@ -2757,7 +2775,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
         <v>211</v>
       </c>
@@ -2789,7 +2807,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
         <v>211</v>
       </c>
@@ -2812,7 +2830,7 @@
       <c r="H69" s="39"/>
       <c r="I69" s="36"/>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
         <v>211</v>
       </c>
@@ -2844,7 +2862,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
         <v>211</v>
       </c>
@@ -2865,7 +2883,7 @@
       </c>
       <c r="G71" s="36"/>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
         <v>211</v>
       </c>
@@ -2886,7 +2904,7 @@
       </c>
       <c r="G72" s="36"/>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
         <v>211</v>
       </c>
@@ -2907,7 +2925,7 @@
       </c>
       <c r="G73" s="36"/>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
         <v>211</v>
       </c>
@@ -2928,7 +2946,7 @@
       </c>
       <c r="G74" s="36"/>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
         <v>211</v>
       </c>
@@ -2949,7 +2967,7 @@
       </c>
       <c r="G75" s="36"/>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
         <v>211</v>
       </c>
@@ -2970,7 +2988,7 @@
       </c>
       <c r="G76" s="36"/>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
         <v>211</v>
       </c>
@@ -2991,7 +3009,7 @@
       </c>
       <c r="G77" s="36"/>
     </row>
-    <row r="78" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:10" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
         <v>211</v>
       </c>
@@ -3012,7 +3030,7 @@
       </c>
       <c r="G78" s="38"/>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
         <v>211</v>
       </c>
@@ -3033,7 +3051,7 @@
       </c>
       <c r="G79" s="36"/>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
         <v>211</v>
       </c>
@@ -3054,7 +3072,7 @@
       </c>
       <c r="G80" s="36"/>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
         <v>211</v>
       </c>
@@ -3086,7 +3104,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
         <v>211</v>
       </c>
@@ -3111,7 +3129,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
         <v>211</v>
       </c>
@@ -3153,7 +3171,7 @@
       </c>
       <c r="G84" s="36"/>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
         <v>211</v>
       </c>
@@ -3174,7 +3192,7 @@
       </c>
       <c r="G85" s="36"/>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
         <v>211</v>
       </c>
@@ -3197,7 +3215,7 @@
       <c r="I86" s="40"/>
       <c r="K86" s="15"/>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
         <v>211</v>
       </c>
@@ -3222,7 +3240,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
         <v>160</v>
       </c>
@@ -3243,7 +3261,7 @@
       </c>
       <c r="G88" s="36"/>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
         <v>160</v>
       </c>
@@ -3264,7 +3282,7 @@
       </c>
       <c r="G89" s="36"/>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
         <v>160</v>
       </c>
@@ -3285,7 +3303,7 @@
       </c>
       <c r="G90" s="36"/>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
         <v>160</v>
       </c>
@@ -3306,7 +3324,7 @@
       </c>
       <c r="G91" s="36"/>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
         <v>160</v>
       </c>
@@ -3327,7 +3345,7 @@
       </c>
       <c r="G92" s="36"/>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
         <v>160</v>
       </c>
@@ -3348,7 +3366,7 @@
       </c>
       <c r="G93" s="36"/>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
         <v>160</v>
       </c>
@@ -3369,7 +3387,7 @@
       </c>
       <c r="G94" s="36"/>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
         <v>160</v>
       </c>
@@ -3390,7 +3408,7 @@
       </c>
       <c r="G95" s="36"/>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
         <v>160</v>
       </c>
@@ -3411,7 +3429,7 @@
       </c>
       <c r="G96" s="36"/>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
         <v>160</v>
       </c>
@@ -3432,7 +3450,7 @@
       </c>
       <c r="G97" s="36"/>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
         <v>160</v>
       </c>
@@ -3453,7 +3471,7 @@
       </c>
       <c r="G98" s="36"/>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
         <v>160</v>
       </c>
@@ -3474,7 +3492,7 @@
       </c>
       <c r="G99" s="36"/>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
         <v>160</v>
       </c>
@@ -3495,7 +3513,7 @@
       </c>
       <c r="G100" s="36"/>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
         <v>160</v>
       </c>
@@ -3516,7 +3534,7 @@
       </c>
       <c r="G101" s="36"/>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="s">
         <v>160</v>
       </c>
@@ -3537,7 +3555,7 @@
       </c>
       <c r="G102" s="36"/>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="s">
         <v>160</v>
       </c>
@@ -3561,7 +3579,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" s="2" t="s">
         <v>160</v>
       </c>
@@ -3582,7 +3600,7 @@
       </c>
       <c r="G104" s="36"/>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="s">
         <v>160</v>
       </c>
@@ -3607,7 +3625,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" s="2" t="s">
         <v>160</v>
       </c>
@@ -3628,7 +3646,7 @@
       </c>
       <c r="G106" s="36"/>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
         <v>160</v>
       </c>
@@ -3649,7 +3667,7 @@
       </c>
       <c r="G107" s="36"/>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="s">
         <v>160</v>
       </c>
@@ -3670,7 +3688,7 @@
       </c>
       <c r="G108" s="36"/>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109" s="2" t="s">
         <v>160</v>
       </c>
@@ -3691,7 +3709,7 @@
       </c>
       <c r="G109" s="36"/>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110" s="28" t="s">
         <v>160</v>
       </c>
@@ -3777,7 +3795,7 @@
       </c>
       <c r="G113" s="36"/>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114" s="10" t="s">
         <v>4</v>
       </c>
@@ -3798,7 +3816,7 @@
       </c>
       <c r="G114" s="36"/>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115" s="10" t="s">
         <v>4</v>
       </c>
@@ -3819,7 +3837,7 @@
       </c>
       <c r="G115" s="36"/>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116" s="10" t="s">
         <v>4</v>
       </c>
@@ -3872,7 +3890,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118" s="12" t="s">
         <v>4</v>
       </c>
@@ -3893,7 +3911,7 @@
       </c>
       <c r="G118" s="36"/>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A119" s="10" t="s">
         <v>4</v>
       </c>
@@ -3914,7 +3932,7 @@
       </c>
       <c r="G119" s="36"/>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120" s="10" t="s">
         <v>4</v>
       </c>
@@ -4012,7 +4030,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="124" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:10" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A124" s="15" t="s">
         <v>4</v>
       </c>
@@ -4033,7 +4051,7 @@
       </c>
       <c r="G124" s="38"/>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A125" s="10" t="s">
         <v>4</v>
       </c>
@@ -4054,7 +4072,7 @@
       </c>
       <c r="G125" s="36"/>
     </row>
-    <row r="126" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:10" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A126" s="15" t="s">
         <v>4</v>
       </c>
@@ -4075,7 +4093,7 @@
       </c>
       <c r="G126" s="38"/>
     </row>
-    <row r="127" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:10" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A127" s="15" t="s">
         <v>4</v>
       </c>
@@ -4096,7 +4114,7 @@
       </c>
       <c r="G127" s="38"/>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A128" s="10" t="s">
         <v>4</v>
       </c>
@@ -4117,7 +4135,7 @@
       </c>
       <c r="G128" s="36"/>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A129" s="10" t="s">
         <v>4</v>
       </c>
@@ -4138,7 +4156,7 @@
       </c>
       <c r="G129" s="36"/>
     </row>
-    <row r="130" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:10" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A130" s="15" t="s">
         <v>4</v>
       </c>
@@ -4159,7 +4177,7 @@
       </c>
       <c r="G130" s="40"/>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A131" s="10" t="s">
         <v>4</v>
       </c>
@@ -4180,7 +4198,7 @@
       </c>
       <c r="G131" s="36"/>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A132" s="10" t="s">
         <v>4</v>
       </c>
@@ -4201,7 +4219,7 @@
       </c>
       <c r="G132" s="36"/>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A133" s="10" t="s">
         <v>4</v>
       </c>
@@ -4254,7 +4272,7 @@
       </c>
       <c r="G134" s="36"/>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A135" s="10" t="s">
         <v>4</v>
       </c>
@@ -4275,7 +4293,7 @@
       </c>
       <c r="G135" s="36"/>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A136" s="10" t="s">
         <v>4</v>
       </c>
@@ -4296,7 +4314,7 @@
       </c>
       <c r="G136" s="36"/>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A137" s="10" t="s">
         <v>4</v>
       </c>
@@ -4317,7 +4335,7 @@
       </c>
       <c r="G137" s="36"/>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A138" s="10" t="s">
         <v>4</v>
       </c>
@@ -4338,7 +4356,7 @@
       </c>
       <c r="G138" s="36"/>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A139" s="10" t="s">
         <v>4</v>
       </c>
@@ -4370,7 +4388,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A140" s="12" t="s">
         <v>4</v>
       </c>
@@ -4412,7 +4430,7 @@
       </c>
       <c r="G141" s="36"/>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A142" s="10" t="s">
         <v>4</v>
       </c>
@@ -4433,7 +4451,7 @@
       </c>
       <c r="G142" s="36"/>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A143" s="12" t="s">
         <v>4</v>
       </c>
@@ -4496,7 +4514,7 @@
       </c>
       <c r="G145" s="36"/>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A146" s="27" t="s">
         <v>4</v>
       </c>
@@ -4538,7 +4556,7 @@
       </c>
       <c r="G147" s="36"/>
     </row>
-    <row r="148" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:11" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A148" s="10" t="s">
         <v>4</v>
       </c>
@@ -4563,7 +4581,7 @@
       <c r="J148" s="37"/>
       <c r="K148" s="10"/>
     </row>
-    <row r="149" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:11" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A149" s="10" t="s">
         <v>4</v>
       </c>
@@ -4588,7 +4606,7 @@
       <c r="J149" s="37"/>
       <c r="K149" s="10"/>
     </row>
-    <row r="150" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:11" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A150" s="27" t="s">
         <v>4</v>
       </c>
@@ -4613,7 +4631,7 @@
       <c r="J150" s="37"/>
       <c r="K150" s="10"/>
     </row>
-    <row r="151" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:11" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A151" s="10" t="s">
         <v>4</v>
       </c>
@@ -4638,7 +4656,7 @@
       <c r="J151" s="37"/>
       <c r="K151" s="10"/>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A152" s="10" t="s">
         <v>4</v>
       </c>
@@ -4670,7 +4688,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A153" s="27" t="s">
         <v>4</v>
       </c>
@@ -4691,7 +4709,7 @@
       </c>
       <c r="G153" s="36"/>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A154" s="10" t="s">
         <v>4</v>
       </c>
@@ -4712,7 +4730,7 @@
       </c>
       <c r="G154" s="36"/>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A155" s="10" t="s">
         <v>4</v>
       </c>
@@ -4733,7 +4751,7 @@
       </c>
       <c r="G155" s="36"/>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A156" s="10" t="s">
         <v>4</v>
       </c>
@@ -4754,7 +4772,7 @@
       </c>
       <c r="G156" s="36"/>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A157" s="10" t="s">
         <v>4</v>
       </c>
@@ -4796,7 +4814,7 @@
       </c>
       <c r="G158" s="36"/>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A159" s="10" t="s">
         <v>4</v>
       </c>
@@ -4817,7 +4835,7 @@
       </c>
       <c r="G159" s="36"/>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A160" s="10" t="s">
         <v>4</v>
       </c>
@@ -4859,7 +4877,7 @@
       </c>
       <c r="G161" s="36"/>
     </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A162" s="10" t="s">
         <v>4</v>
       </c>
@@ -4880,7 +4898,7 @@
       </c>
       <c r="G162" s="36"/>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A163" s="10" t="s">
         <v>4</v>
       </c>
@@ -4901,7 +4919,7 @@
       </c>
       <c r="G163" s="36"/>
     </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A164" s="10" t="s">
         <v>4</v>
       </c>
@@ -4922,7 +4940,7 @@
       </c>
       <c r="G164" s="36"/>
     </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A165" s="10" t="s">
         <v>4</v>
       </c>
@@ -4954,7 +4972,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A166" s="10" t="s">
         <v>4</v>
       </c>
@@ -4986,7 +5004,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A167" s="10" t="s">
         <v>4</v>
       </c>
@@ -5007,7 +5025,7 @@
       </c>
       <c r="G167" s="36"/>
     </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A168" s="10" t="s">
         <v>4</v>
       </c>
@@ -5028,7 +5046,7 @@
       </c>
       <c r="G168" s="36"/>
     </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A169" s="10" t="s">
         <v>4</v>
       </c>
@@ -5049,7 +5067,7 @@
       </c>
       <c r="G169" s="36"/>
     </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A170" s="10" t="s">
         <v>4</v>
       </c>
@@ -5091,7 +5109,7 @@
       </c>
       <c r="G171" s="36"/>
     </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A172" s="10" t="s">
         <v>4</v>
       </c>
@@ -5112,7 +5130,7 @@
       </c>
       <c r="G172" s="36"/>
     </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A173" s="10" t="s">
         <v>4</v>
       </c>
@@ -5133,7 +5151,7 @@
       </c>
       <c r="G173" s="36"/>
     </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A174" s="12" t="s">
         <v>4</v>
       </c>
@@ -5186,7 +5204,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A176" s="10" t="s">
         <v>4</v>
       </c>
@@ -5228,7 +5246,7 @@
       </c>
       <c r="G177" s="36"/>
     </row>
-    <row r="178" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A178" s="10" t="s">
         <v>4</v>
       </c>
@@ -5249,7 +5267,7 @@
       </c>
       <c r="G178" s="36"/>
     </row>
-    <row r="179" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A179" s="10" t="s">
         <v>4</v>
       </c>
@@ -5291,7 +5309,7 @@
       </c>
       <c r="G180" s="36"/>
     </row>
-    <row r="181" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A181" s="10" t="s">
         <v>4</v>
       </c>
@@ -5323,7 +5341,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="182" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A182" s="10" t="s">
         <v>4</v>
       </c>
@@ -5388,7 +5406,7 @@
       </c>
       <c r="K183" s="12"/>
     </row>
-    <row r="184" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:11" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A184" s="15" t="s">
         <v>4</v>
       </c>
@@ -5409,7 +5427,7 @@
       </c>
       <c r="G184" s="38"/>
     </row>
-    <row r="185" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A185" s="10" t="s">
         <v>4</v>
       </c>
@@ -5430,7 +5448,7 @@
       </c>
       <c r="G185" s="36"/>
     </row>
-    <row r="186" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:11" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A186" s="15" t="s">
         <v>4</v>
       </c>
@@ -5451,7 +5469,7 @@
       </c>
       <c r="G186" s="38"/>
     </row>
-    <row r="187" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:11" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A187" s="15" t="s">
         <v>4</v>
       </c>
@@ -5472,7 +5490,7 @@
       </c>
       <c r="G187" s="38"/>
     </row>
-    <row r="188" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A188" s="10" t="s">
         <v>4</v>
       </c>
@@ -5493,7 +5511,7 @@
       </c>
       <c r="G188" s="36"/>
     </row>
-    <row r="189" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A189" s="10" t="s">
         <v>4</v>
       </c>
@@ -5514,7 +5532,7 @@
       </c>
       <c r="G189" s="36"/>
     </row>
-    <row r="190" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A190" s="10" t="s">
         <v>4</v>
       </c>
@@ -5535,7 +5553,7 @@
       </c>
       <c r="G190" s="36"/>
     </row>
-    <row r="191" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A191" s="10" t="s">
         <v>4</v>
       </c>
@@ -5567,7 +5585,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="192" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A192" s="10" t="s">
         <v>4</v>
       </c>
@@ -5599,7 +5617,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="193" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A193" s="10" t="s">
         <v>4</v>
       </c>
@@ -5620,7 +5638,7 @@
       </c>
       <c r="G193" s="36"/>
     </row>
-    <row r="194" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:11" ht="16" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A194" s="10" t="s">
         <v>4</v>
       </c>
@@ -5641,7 +5659,7 @@
       </c>
       <c r="G194" s="36"/>
     </row>
-    <row r="195" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:11" ht="16" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A195" s="10" t="s">
         <v>4</v>
       </c>
@@ -5662,7 +5680,7 @@
       </c>
       <c r="G195" s="36"/>
     </row>
-    <row r="196" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:11" ht="16" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A196" s="10" t="s">
         <v>4</v>
       </c>
@@ -5683,7 +5701,7 @@
       </c>
       <c r="G196" s="36"/>
     </row>
-    <row r="197" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:11" ht="16" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A197" s="18" t="s">
         <v>4</v>
       </c>
@@ -5747,7 +5765,7 @@
       </c>
       <c r="G199" s="36"/>
     </row>
-    <row r="200" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:11" ht="16" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A200" s="18" t="s">
         <v>4</v>
       </c>
@@ -5768,7 +5786,7 @@
       </c>
       <c r="G200" s="36"/>
     </row>
-    <row r="201" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:11" ht="16" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A201" s="18" t="s">
         <v>4</v>
       </c>
@@ -5789,7 +5807,7 @@
       </c>
       <c r="G201" s="36"/>
     </row>
-    <row r="202" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:11" ht="16" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A202" s="18" t="s">
         <v>4</v>
       </c>
@@ -5831,7 +5849,7 @@
       </c>
       <c r="G203" s="36"/>
     </row>
-    <row r="204" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:11" ht="16" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A204" s="18" t="s">
         <v>4</v>
       </c>
@@ -5853,7 +5871,7 @@
       <c r="G204" s="36"/>
       <c r="K204" s="51"/>
     </row>
-    <row r="205" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:11" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A205" s="13" t="s">
         <v>4</v>
       </c>
@@ -5927,7 +5945,7 @@
       <c r="I207" s="40"/>
       <c r="K207" s="51"/>
     </row>
-    <row r="208" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:11" ht="16" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A208" s="18" t="s">
         <v>4</v>
       </c>
@@ -5950,7 +5968,7 @@
       <c r="I208" s="40"/>
       <c r="K208" s="35"/>
     </row>
-    <row r="209" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:11" ht="16" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A209" s="18" t="s">
         <v>4</v>
       </c>
@@ -5973,8 +5991,34 @@
       <c r="I209" s="40"/>
       <c r="K209" s="35"/>
     </row>
+    <row r="210" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A210" s="52" t="s">
+        <v>4</v>
+      </c>
+      <c r="B210" s="53" t="s">
+        <v>34</v>
+      </c>
+      <c r="C210" s="53" t="s">
+        <v>46</v>
+      </c>
+      <c r="D210" s="54" t="s">
+        <v>187</v>
+      </c>
+      <c r="E210" s="53" t="s">
+        <v>212</v>
+      </c>
+      <c r="F210" s="54" t="s">
+        <v>187</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:K1" xr:uid="{749F81FE-5A40-422C-A0CF-574E71A9CE1E}"/>
+  <autoFilter ref="A1:K210" xr:uid="{749F81FE-5A40-422C-A0CF-574E71A9CE1E}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Other Soil Properties"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K209">
     <sortCondition ref="A2:A209"/>
   </sortState>

</xml_diff>

<commit_message>
Move labile carbon and isotopes to other soil properties
</commit_message>
<xml_diff>
--- a/data/normative-effects.xlsx
+++ b/data/normative-effects.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephen.wood/Box Sync/Work/The Nature Conservancy/Global Soils/AgEvidence/code-and-data/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4122DAAD-04F3-184A-9425-D4D4E66EC2F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6903CF44-C3F5-4C41-96DD-29D8E13A8FE6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2520" yWindow="460" windowWidth="19200" windowHeight="14560" xr2:uid="{E2614878-5E79-439B-BF47-44ECB7DBED54}"/>
+    <workbookView xWindow="2520" yWindow="460" windowWidth="23900" windowHeight="14560" xr2:uid="{E2614878-5E79-439B-BF47-44ECB7DBED54}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1369" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1387" uniqueCount="215">
   <si>
     <t>Review</t>
   </si>
@@ -667,13 +667,19 @@
   </si>
   <si>
     <t>Methane oxidation</t>
+  </si>
+  <si>
+    <t>Labile carbon</t>
+  </si>
+  <si>
+    <t>Natural abundance of 13C</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -694,6 +700,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Lucida Grande"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -818,7 +830,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
@@ -902,6 +914,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1219,12 +1232,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5790928A-FDEF-4501-A63F-C28CBDB4D383}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:K210"/>
+  <dimension ref="A1:K213"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="F210" sqref="F210"/>
+      <selection pane="bottomLeft" activeCell="E214" sqref="E214"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1278,7 +1291,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
         <v>190</v>
       </c>
@@ -1301,7 +1314,7 @@
       <c r="H2" s="36"/>
       <c r="I2" s="36"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
         <v>190</v>
       </c>
@@ -1322,7 +1335,7 @@
       </c>
       <c r="G3" s="36"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
         <v>190</v>
       </c>
@@ -1388,7 +1401,7 @@
       </c>
       <c r="G6" s="36"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
         <v>190</v>
       </c>
@@ -1430,7 +1443,7 @@
       </c>
       <c r="G8" s="36"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
         <v>190</v>
       </c>
@@ -1662,7 +1675,7 @@
       </c>
       <c r="G18" s="36"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="11" t="s">
         <v>190</v>
       </c>
@@ -1683,7 +1696,7 @@
       </c>
       <c r="G19" s="36"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>190</v>
       </c>
@@ -1894,7 +1907,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="11" t="s">
         <v>190</v>
       </c>
@@ -2104,7 +2117,7 @@
       </c>
       <c r="G38" s="36"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="11" t="s">
         <v>190</v>
       </c>
@@ -2146,7 +2159,7 @@
       </c>
       <c r="G40" s="36"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="11" t="s">
         <v>190</v>
       </c>
@@ -2167,7 +2180,7 @@
       </c>
       <c r="G41" s="36"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="11" t="s">
         <v>190</v>
       </c>
@@ -2191,7 +2204,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="11" t="s">
         <v>190</v>
       </c>
@@ -2277,7 +2290,7 @@
       </c>
       <c r="K45" s="12"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" s="11" t="s">
         <v>190</v>
       </c>
@@ -2426,7 +2439,7 @@
       </c>
       <c r="G52" s="36"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" s="11" t="s">
         <v>190</v>
       </c>
@@ -2470,7 +2483,7 @@
       <c r="H54" s="40"/>
       <c r="I54" s="40"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" s="11" t="s">
         <v>190</v>
       </c>
@@ -3150,7 +3163,7 @@
       </c>
       <c r="G83" s="36"/>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
         <v>211</v>
       </c>
@@ -3732,7 +3745,7 @@
       <c r="H110" s="40"/>
       <c r="I110" s="40"/>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111" s="12" t="s">
         <v>4</v>
       </c>
@@ -3753,7 +3766,7 @@
       </c>
       <c r="G111" s="36"/>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112" s="12" t="s">
         <v>4</v>
       </c>
@@ -3774,7 +3787,7 @@
       </c>
       <c r="G112" s="36"/>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113" s="12" t="s">
         <v>4</v>
       </c>
@@ -3858,7 +3871,7 @@
       </c>
       <c r="G116" s="36"/>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A117" s="12" t="s">
         <v>4</v>
       </c>
@@ -3977,7 +3990,7 @@
       <c r="I121" s="36"/>
       <c r="J121" s="36"/>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A122" s="10" t="s">
         <v>4</v>
       </c>
@@ -3998,7 +4011,7 @@
       </c>
       <c r="G122" s="36"/>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A123" s="10" t="s">
         <v>4</v>
       </c>
@@ -4251,7 +4264,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A134" s="10" t="s">
         <v>4</v>
       </c>
@@ -4409,7 +4422,7 @@
       </c>
       <c r="G140" s="36"/>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A141" s="12" t="s">
         <v>4</v>
       </c>
@@ -4472,7 +4485,7 @@
       </c>
       <c r="G143" s="36"/>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A144" s="10" t="s">
         <v>4</v>
       </c>
@@ -4493,7 +4506,7 @@
       </c>
       <c r="G144" s="36"/>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A145" s="10" t="s">
         <v>4</v>
       </c>
@@ -4535,7 +4548,7 @@
       </c>
       <c r="G146" s="36"/>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A147" s="12" t="s">
         <v>4</v>
       </c>
@@ -4793,7 +4806,7 @@
       </c>
       <c r="G157" s="36"/>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A158" s="12" t="s">
         <v>4</v>
       </c>
@@ -4856,7 +4869,7 @@
       </c>
       <c r="G160" s="36"/>
     </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A161" s="10" t="s">
         <v>4</v>
       </c>
@@ -5172,7 +5185,7 @@
       </c>
       <c r="G174" s="36"/>
     </row>
-    <row r="175" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:10" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A175" s="15" t="s">
         <v>4</v>
       </c>
@@ -5225,7 +5238,7 @@
       </c>
       <c r="G176" s="36"/>
     </row>
-    <row r="177" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A177" s="10" t="s">
         <v>4</v>
       </c>
@@ -5288,7 +5301,7 @@
       </c>
       <c r="G179" s="36"/>
     </row>
-    <row r="180" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A180" s="10" t="s">
         <v>4</v>
       </c>
@@ -5617,7 +5630,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="193" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A193" s="10" t="s">
         <v>4</v>
       </c>
@@ -5638,7 +5651,7 @@
       </c>
       <c r="G193" s="36"/>
     </row>
-    <row r="194" spans="1:11" ht="16" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A194" s="10" t="s">
         <v>4</v>
       </c>
@@ -5659,7 +5672,7 @@
       </c>
       <c r="G194" s="36"/>
     </row>
-    <row r="195" spans="1:11" ht="16" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A195" s="10" t="s">
         <v>4</v>
       </c>
@@ -5680,7 +5693,7 @@
       </c>
       <c r="G195" s="36"/>
     </row>
-    <row r="196" spans="1:11" ht="16" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A196" s="10" t="s">
         <v>4</v>
       </c>
@@ -5723,7 +5736,7 @@
       <c r="G197" s="36"/>
       <c r="K197" s="51"/>
     </row>
-    <row r="198" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:11" ht="16" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A198" s="18" t="s">
         <v>4</v>
       </c>
@@ -5744,7 +5757,7 @@
       </c>
       <c r="G198" s="36"/>
     </row>
-    <row r="199" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:11" ht="16" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A199" s="18" t="s">
         <v>4</v>
       </c>
@@ -5828,7 +5841,7 @@
       </c>
       <c r="G202" s="36"/>
     </row>
-    <row r="203" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:11" ht="16" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A203" s="16" t="s">
         <v>4</v>
       </c>
@@ -5897,7 +5910,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="206" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:11" ht="16" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A206" s="18" t="s">
         <v>4</v>
       </c>
@@ -5921,7 +5934,7 @@
       <c r="I206" s="40"/>
       <c r="K206" s="51"/>
     </row>
-    <row r="207" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:11" ht="16" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A207" s="16" t="s">
         <v>4</v>
       </c>
@@ -5991,7 +6004,7 @@
       <c r="I209" s="40"/>
       <c r="K209" s="35"/>
     </row>
-    <row r="210" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A210" s="52" t="s">
         <v>4</v>
       </c>
@@ -6009,6 +6022,66 @@
       </c>
       <c r="F210" s="54" t="s">
         <v>187</v>
+      </c>
+    </row>
+    <row r="211" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A211" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="B211" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C211" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D211" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="E211" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="F211" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="212" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A212" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B212" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C212" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D212" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="E212" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="F212" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="213" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A213" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B213" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C213" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D213" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="E213" s="55" t="s">
+        <v>214</v>
+      </c>
+      <c r="F213" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -6016,6 +6089,11 @@
     <filterColumn colId="1">
       <filters>
         <filter val="Other Soil Properties"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="2">
+      <filters>
+        <filter val="Chemical Properties"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
Move C erosion from climate to other soil properties
</commit_message>
<xml_diff>
--- a/data/normative-effects.xlsx
+++ b/data/normative-effects.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephen.wood/Box Sync/Work/The Nature Conservancy/Global Soils/AgEvidence/code-and-data/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F28A9292-567C-B94D-8A35-B8E3CB707505}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB274283-C69A-1845-82B7-194D45917699}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2520" yWindow="460" windowWidth="23900" windowHeight="14560" xr2:uid="{E2614878-5E79-439B-BF47-44ECB7DBED54}"/>
+    <workbookView xWindow="2520" yWindow="460" windowWidth="19200" windowHeight="14560" xr2:uid="{E2614878-5E79-439B-BF47-44ECB7DBED54}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1387" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1369" uniqueCount="213">
   <si>
     <t>Review</t>
   </si>
@@ -667,19 +667,13 @@
   </si>
   <si>
     <t>Methane oxidation</t>
-  </si>
-  <si>
-    <t>Labile carbon</t>
-  </si>
-  <si>
-    <t>Natural abundance of 13C</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -700,12 +694,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Lucida Grande"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -830,7 +818,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
@@ -914,7 +902,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1232,12 +1219,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5790928A-FDEF-4501-A63F-C28CBDB4D383}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:K213"/>
+  <dimension ref="A1:K210"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="E214" sqref="E214"/>
+      <selection pane="bottomLeft" activeCell="F210" sqref="F210"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1291,7 +1278,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="2" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
         <v>190</v>
       </c>
@@ -1314,7 +1301,7 @@
       <c r="H2" s="36"/>
       <c r="I2" s="36"/>
     </row>
-    <row r="3" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
         <v>190</v>
       </c>
@@ -1335,7 +1322,7 @@
       </c>
       <c r="G3" s="36"/>
     </row>
-    <row r="4" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
         <v>190</v>
       </c>
@@ -1401,7 +1388,7 @@
       </c>
       <c r="G6" s="36"/>
     </row>
-    <row r="7" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
         <v>190</v>
       </c>
@@ -1443,7 +1430,7 @@
       </c>
       <c r="G8" s="36"/>
     </row>
-    <row r="9" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
         <v>190</v>
       </c>
@@ -1675,7 +1662,7 @@
       </c>
       <c r="G18" s="36"/>
     </row>
-    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="11" t="s">
         <v>190</v>
       </c>
@@ -1696,7 +1683,7 @@
       </c>
       <c r="G19" s="36"/>
     </row>
-    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>190</v>
       </c>
@@ -1907,7 +1894,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="11" t="s">
         <v>190</v>
       </c>
@@ -2117,7 +2104,7 @@
       </c>
       <c r="G38" s="36"/>
     </row>
-    <row r="39" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="11" t="s">
         <v>190</v>
       </c>
@@ -2159,7 +2146,7 @@
       </c>
       <c r="G40" s="36"/>
     </row>
-    <row r="41" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" s="11" t="s">
         <v>190</v>
       </c>
@@ -2180,7 +2167,7 @@
       </c>
       <c r="G41" s="36"/>
     </row>
-    <row r="42" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" s="11" t="s">
         <v>190</v>
       </c>
@@ -2204,7 +2191,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="43" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" s="11" t="s">
         <v>190</v>
       </c>
@@ -2290,7 +2277,7 @@
       </c>
       <c r="K45" s="12"/>
     </row>
-    <row r="46" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" s="11" t="s">
         <v>190</v>
       </c>
@@ -2439,7 +2426,7 @@
       </c>
       <c r="G52" s="36"/>
     </row>
-    <row r="53" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" s="11" t="s">
         <v>190</v>
       </c>
@@ -2483,7 +2470,7 @@
       <c r="H54" s="40"/>
       <c r="I54" s="40"/>
     </row>
-    <row r="55" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" s="11" t="s">
         <v>190</v>
       </c>
@@ -3163,7 +3150,7 @@
       </c>
       <c r="G83" s="36"/>
     </row>
-    <row r="84" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
         <v>211</v>
       </c>
@@ -3745,7 +3732,7 @@
       <c r="H110" s="40"/>
       <c r="I110" s="40"/>
     </row>
-    <row r="111" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A111" s="12" t="s">
         <v>4</v>
       </c>
@@ -3766,7 +3753,7 @@
       </c>
       <c r="G111" s="36"/>
     </row>
-    <row r="112" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A112" s="12" t="s">
         <v>4</v>
       </c>
@@ -3787,7 +3774,7 @@
       </c>
       <c r="G112" s="36"/>
     </row>
-    <row r="113" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A113" s="12" t="s">
         <v>4</v>
       </c>
@@ -3871,7 +3858,7 @@
       </c>
       <c r="G116" s="36"/>
     </row>
-    <row r="117" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A117" s="12" t="s">
         <v>4</v>
       </c>
@@ -3990,7 +3977,7 @@
       <c r="I121" s="36"/>
       <c r="J121" s="36"/>
     </row>
-    <row r="122" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A122" s="10" t="s">
         <v>4</v>
       </c>
@@ -4011,7 +3998,7 @@
       </c>
       <c r="G122" s="36"/>
     </row>
-    <row r="123" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A123" s="10" t="s">
         <v>4</v>
       </c>
@@ -4264,7 +4251,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="134" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A134" s="10" t="s">
         <v>4</v>
       </c>
@@ -4422,7 +4409,7 @@
       </c>
       <c r="G140" s="36"/>
     </row>
-    <row r="141" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A141" s="12" t="s">
         <v>4</v>
       </c>
@@ -4485,7 +4472,7 @@
       </c>
       <c r="G143" s="36"/>
     </row>
-    <row r="144" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A144" s="10" t="s">
         <v>4</v>
       </c>
@@ -4506,7 +4493,7 @@
       </c>
       <c r="G144" s="36"/>
     </row>
-    <row r="145" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A145" s="10" t="s">
         <v>4</v>
       </c>
@@ -4548,7 +4535,7 @@
       </c>
       <c r="G146" s="36"/>
     </row>
-    <row r="147" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A147" s="12" t="s">
         <v>4</v>
       </c>
@@ -4806,7 +4793,7 @@
       </c>
       <c r="G157" s="36"/>
     </row>
-    <row r="158" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A158" s="12" t="s">
         <v>4</v>
       </c>
@@ -4869,7 +4856,7 @@
       </c>
       <c r="G160" s="36"/>
     </row>
-    <row r="161" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A161" s="10" t="s">
         <v>4</v>
       </c>
@@ -5185,7 +5172,7 @@
       </c>
       <c r="G174" s="36"/>
     </row>
-    <row r="175" spans="1:10" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A175" s="15" t="s">
         <v>4</v>
       </c>
@@ -5238,7 +5225,7 @@
       </c>
       <c r="G176" s="36"/>
     </row>
-    <row r="177" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A177" s="10" t="s">
         <v>4</v>
       </c>
@@ -5301,7 +5288,7 @@
       </c>
       <c r="G179" s="36"/>
     </row>
-    <row r="180" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A180" s="10" t="s">
         <v>4</v>
       </c>
@@ -5630,7 +5617,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="193" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A193" s="10" t="s">
         <v>4</v>
       </c>
@@ -5651,7 +5638,7 @@
       </c>
       <c r="G193" s="36"/>
     </row>
-    <row r="194" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:11" ht="16" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A194" s="10" t="s">
         <v>4</v>
       </c>
@@ -5672,7 +5659,7 @@
       </c>
       <c r="G194" s="36"/>
     </row>
-    <row r="195" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:11" ht="16" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A195" s="10" t="s">
         <v>4</v>
       </c>
@@ -5693,7 +5680,7 @@
       </c>
       <c r="G195" s="36"/>
     </row>
-    <row r="196" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:11" ht="16" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A196" s="10" t="s">
         <v>4</v>
       </c>
@@ -5736,7 +5723,7 @@
       <c r="G197" s="36"/>
       <c r="K197" s="51"/>
     </row>
-    <row r="198" spans="1:11" ht="16" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A198" s="18" t="s">
         <v>4</v>
       </c>
@@ -5757,7 +5744,7 @@
       </c>
       <c r="G198" s="36"/>
     </row>
-    <row r="199" spans="1:11" ht="16" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A199" s="18" t="s">
         <v>4</v>
       </c>
@@ -5841,7 +5828,7 @@
       </c>
       <c r="G202" s="36"/>
     </row>
-    <row r="203" spans="1:11" ht="16" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A203" s="16" t="s">
         <v>4</v>
       </c>
@@ -5910,7 +5897,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="206" spans="1:11" ht="16" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A206" s="18" t="s">
         <v>4</v>
       </c>
@@ -5934,7 +5921,7 @@
       <c r="I206" s="40"/>
       <c r="K206" s="51"/>
     </row>
-    <row r="207" spans="1:11" ht="16" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A207" s="16" t="s">
         <v>4</v>
       </c>
@@ -6004,7 +5991,7 @@
       <c r="I209" s="40"/>
       <c r="K209" s="35"/>
     </row>
-    <row r="210" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A210" s="52" t="s">
         <v>4</v>
       </c>
@@ -6022,66 +6009,6 @@
       </c>
       <c r="F210" s="54" t="s">
         <v>187</v>
-      </c>
-    </row>
-    <row r="211" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A211" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="B211" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C211" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D211" s="7" t="s">
-        <v>187</v>
-      </c>
-      <c r="E211" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="F211" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="212" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A212" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B212" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C212" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D212" s="7" t="s">
-        <v>187</v>
-      </c>
-      <c r="E212" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="F212" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="213" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A213" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B213" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C213" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D213" s="7" t="s">
-        <v>187</v>
-      </c>
-      <c r="E213" s="55" t="s">
-        <v>214</v>
-      </c>
-      <c r="F213" s="1" t="s">
-        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -6089,11 +6016,6 @@
     <filterColumn colId="1">
       <filters>
         <filter val="Other Soil Properties"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="2">
-      <filters>
-        <filter val="Chemical Properties"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
Resolved NA problems in new GL3s
</commit_message>
<xml_diff>
--- a/data/normative-effects.xlsx
+++ b/data/normative-effects.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephen.wood/Box Sync/Work/The Nature Conservancy/Global Soils/AgEvidence/code-and-data/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB274283-C69A-1845-82B7-194D45917699}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C44D25B1-C3B2-7843-8FCB-33A4DBF0B5E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2520" yWindow="460" windowWidth="19200" windowHeight="14560" xr2:uid="{E2614878-5E79-439B-BF47-44ECB7DBED54}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$K$210</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1369" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1393" uniqueCount="215">
   <si>
     <t>Review</t>
   </si>
@@ -667,6 +667,12 @@
   </si>
   <si>
     <t>Methane oxidation</t>
+  </si>
+  <si>
+    <t>Labile Carbon</t>
+  </si>
+  <si>
+    <t>Natural Abundance of 13C</t>
   </si>
 </sst>
 </file>
@@ -1219,12 +1225,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5790928A-FDEF-4501-A63F-C28CBDB4D383}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:K210"/>
+  <dimension ref="A1:K214"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="F210" sqref="F210"/>
+      <selection pane="bottomLeft" activeCell="D214" sqref="D214"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1278,7 +1284,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
         <v>190</v>
       </c>
@@ -1301,7 +1307,7 @@
       <c r="H2" s="36"/>
       <c r="I2" s="36"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
         <v>190</v>
       </c>
@@ -1322,7 +1328,7 @@
       </c>
       <c r="G3" s="36"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
         <v>190</v>
       </c>
@@ -1388,7 +1394,7 @@
       </c>
       <c r="G6" s="36"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
         <v>190</v>
       </c>
@@ -1430,7 +1436,7 @@
       </c>
       <c r="G8" s="36"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
         <v>190</v>
       </c>
@@ -1662,7 +1668,7 @@
       </c>
       <c r="G18" s="36"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="11" t="s">
         <v>190</v>
       </c>
@@ -1683,7 +1689,7 @@
       </c>
       <c r="G19" s="36"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>190</v>
       </c>
@@ -1894,7 +1900,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="11" t="s">
         <v>190</v>
       </c>
@@ -2104,7 +2110,7 @@
       </c>
       <c r="G38" s="36"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="11" t="s">
         <v>190</v>
       </c>
@@ -2146,7 +2152,7 @@
       </c>
       <c r="G40" s="36"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="11" t="s">
         <v>190</v>
       </c>
@@ -2167,7 +2173,7 @@
       </c>
       <c r="G41" s="36"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="11" t="s">
         <v>190</v>
       </c>
@@ -2191,7 +2197,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="11" t="s">
         <v>190</v>
       </c>
@@ -2277,7 +2283,7 @@
       </c>
       <c r="K45" s="12"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" s="11" t="s">
         <v>190</v>
       </c>
@@ -2426,7 +2432,7 @@
       </c>
       <c r="G52" s="36"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" s="11" t="s">
         <v>190</v>
       </c>
@@ -2470,7 +2476,7 @@
       <c r="H54" s="40"/>
       <c r="I54" s="40"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" s="11" t="s">
         <v>190</v>
       </c>
@@ -3150,7 +3156,7 @@
       </c>
       <c r="G83" s="36"/>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
         <v>211</v>
       </c>
@@ -3732,7 +3738,7 @@
       <c r="H110" s="40"/>
       <c r="I110" s="40"/>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111" s="12" t="s">
         <v>4</v>
       </c>
@@ -3753,7 +3759,7 @@
       </c>
       <c r="G111" s="36"/>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112" s="12" t="s">
         <v>4</v>
       </c>
@@ -3774,7 +3780,7 @@
       </c>
       <c r="G112" s="36"/>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113" s="12" t="s">
         <v>4</v>
       </c>
@@ -3858,7 +3864,7 @@
       </c>
       <c r="G116" s="36"/>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A117" s="12" t="s">
         <v>4</v>
       </c>
@@ -3977,7 +3983,7 @@
       <c r="I121" s="36"/>
       <c r="J121" s="36"/>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A122" s="10" t="s">
         <v>4</v>
       </c>
@@ -3998,7 +4004,7 @@
       </c>
       <c r="G122" s="36"/>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A123" s="10" t="s">
         <v>4</v>
       </c>
@@ -4251,7 +4257,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A134" s="10" t="s">
         <v>4</v>
       </c>
@@ -4409,7 +4415,7 @@
       </c>
       <c r="G140" s="36"/>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A141" s="12" t="s">
         <v>4</v>
       </c>
@@ -4472,7 +4478,7 @@
       </c>
       <c r="G143" s="36"/>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A144" s="10" t="s">
         <v>4</v>
       </c>
@@ -4493,7 +4499,7 @@
       </c>
       <c r="G144" s="36"/>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A145" s="10" t="s">
         <v>4</v>
       </c>
@@ -4535,7 +4541,7 @@
       </c>
       <c r="G146" s="36"/>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A147" s="12" t="s">
         <v>4</v>
       </c>
@@ -4793,7 +4799,7 @@
       </c>
       <c r="G157" s="36"/>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A158" s="12" t="s">
         <v>4</v>
       </c>
@@ -4856,7 +4862,7 @@
       </c>
       <c r="G160" s="36"/>
     </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A161" s="10" t="s">
         <v>4</v>
       </c>
@@ -5172,7 +5178,7 @@
       </c>
       <c r="G174" s="36"/>
     </row>
-    <row r="175" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:10" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A175" s="15" t="s">
         <v>4</v>
       </c>
@@ -5225,7 +5231,7 @@
       </c>
       <c r="G176" s="36"/>
     </row>
-    <row r="177" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A177" s="10" t="s">
         <v>4</v>
       </c>
@@ -5288,7 +5294,7 @@
       </c>
       <c r="G179" s="36"/>
     </row>
-    <row r="180" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A180" s="10" t="s">
         <v>4</v>
       </c>
@@ -5617,7 +5623,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="193" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A193" s="10" t="s">
         <v>4</v>
       </c>
@@ -5638,7 +5644,7 @@
       </c>
       <c r="G193" s="36"/>
     </row>
-    <row r="194" spans="1:11" ht="16" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A194" s="10" t="s">
         <v>4</v>
       </c>
@@ -5659,7 +5665,7 @@
       </c>
       <c r="G194" s="36"/>
     </row>
-    <row r="195" spans="1:11" ht="16" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A195" s="10" t="s">
         <v>4</v>
       </c>
@@ -5680,7 +5686,7 @@
       </c>
       <c r="G195" s="36"/>
     </row>
-    <row r="196" spans="1:11" ht="16" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A196" s="10" t="s">
         <v>4</v>
       </c>
@@ -5723,7 +5729,7 @@
       <c r="G197" s="36"/>
       <c r="K197" s="51"/>
     </row>
-    <row r="198" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:11" ht="16" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A198" s="18" t="s">
         <v>4</v>
       </c>
@@ -5744,7 +5750,7 @@
       </c>
       <c r="G198" s="36"/>
     </row>
-    <row r="199" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:11" ht="16" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A199" s="18" t="s">
         <v>4</v>
       </c>
@@ -5828,7 +5834,7 @@
       </c>
       <c r="G202" s="36"/>
     </row>
-    <row r="203" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:11" ht="16" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A203" s="16" t="s">
         <v>4</v>
       </c>
@@ -5897,7 +5903,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="206" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:11" ht="16" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A206" s="18" t="s">
         <v>4</v>
       </c>
@@ -5921,7 +5927,7 @@
       <c r="I206" s="40"/>
       <c r="K206" s="51"/>
     </row>
-    <row r="207" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:11" ht="16" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A207" s="16" t="s">
         <v>4</v>
       </c>
@@ -5991,7 +5997,7 @@
       <c r="I209" s="40"/>
       <c r="K209" s="35"/>
     </row>
-    <row r="210" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A210" s="52" t="s">
         <v>4</v>
       </c>
@@ -6009,6 +6015,86 @@
       </c>
       <c r="F210" s="54" t="s">
         <v>187</v>
+      </c>
+    </row>
+    <row r="211" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A211" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="B211" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C211" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D211" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="E211" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="F211" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="212" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A212" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B212" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C212" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D212" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="E212" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="F212" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="213" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A213" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B213" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C213" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D213" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="E213" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="F213" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="214" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A214" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="B214" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C214" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D214" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="E214" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="F214" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -6016,6 +6102,11 @@
     <filterColumn colId="1">
       <filters>
         <filter val="Other Soil Properties"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="2">
+      <filters>
+        <filter val="Chemical Properties"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
Fixed normative effect error
</commit_message>
<xml_diff>
--- a/data/normative-effects.xlsx
+++ b/data/normative-effects.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephen.wood/Box Sync/Work/The Nature Conservancy/Global Soils/AgEvidence/code-and-data/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AFC0C7C-F1FD-294A-ACAC-5882CAF2E788}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{585DA4D8-508A-8044-AE07-24FCAE87876B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="560" yWindow="500" windowWidth="26280" windowHeight="16620" xr2:uid="{E2614878-5E79-439B-BF47-44ECB7DBED54}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$K$288</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$K$289</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1328,9 +1328,9 @@
   <dimension ref="A1:K289"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="138" zoomScaleNormal="138" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A115" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A97" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="E290" sqref="E290"/>
+      <selection pane="bottomLeft" activeCell="D290" sqref="D290"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3533,7 +3533,7 @@
       </c>
       <c r="G96" s="36"/>
     </row>
-    <row r="97" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
         <v>128</v>
       </c>
@@ -3708,7 +3708,7 @@
       </c>
       <c r="G104" s="36"/>
     </row>
-    <row r="105" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A105" s="28" t="s">
         <v>128</v>
       </c>
@@ -3931,7 +3931,7 @@
       </c>
       <c r="G114" s="36"/>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115" s="10" t="s">
         <v>4</v>
       </c>
@@ -4725,7 +4725,7 @@
       </c>
       <c r="G149" s="36"/>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A150" s="10" t="s">
         <v>4</v>
       </c>
@@ -4999,7 +4999,7 @@
       </c>
       <c r="G161" s="36"/>
     </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A162" s="10" t="s">
         <v>4</v>
       </c>
@@ -5262,7 +5262,7 @@
       </c>
       <c r="G173" s="36"/>
     </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A174" s="10" t="s">
         <v>4</v>
       </c>
@@ -5294,7 +5294,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A175" s="10" t="s">
         <v>4</v>
       </c>
@@ -6756,7 +6756,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="243" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A243" s="10" t="s">
         <v>128</v>
       </c>
@@ -6766,8 +6766,8 @@
       <c r="C243" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="D243" s="1" t="s">
-        <v>150</v>
+      <c r="D243" s="3" t="s">
+        <v>151</v>
       </c>
       <c r="E243" s="4" t="s">
         <v>81</v>
@@ -6968,7 +6968,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="253" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A253" s="10" t="s">
         <v>4</v>
       </c>
@@ -7448,7 +7448,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="277" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A277" s="10" t="s">
         <v>4</v>
       </c>
@@ -7468,7 +7468,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="278" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A278" s="10" t="s">
         <v>4</v>
       </c>
@@ -7688,7 +7688,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="289" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A289" s="10" t="s">
         <v>4</v>
       </c>
@@ -7709,15 +7709,15 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K288" xr:uid="{8B1360B6-23BC-4F49-9C86-2B3B194A8FE8}">
+  <autoFilter ref="A1:K289" xr:uid="{8B1360B6-23BC-4F49-9C86-2B3B194A8FE8}">
     <filterColumn colId="0">
       <filters>
-        <filter val="Tillage"/>
+        <filter val="Nutrient Management"/>
       </filters>
     </filterColumn>
     <filterColumn colId="1">
       <filters>
-        <filter val="Climate Mitigation"/>
+        <filter val="Water Quality"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>